<commit_message>
Created convert coordinate to node. Dfs fully functional
</commit_message>
<xml_diff>
--- a/MatrixSample.xlsx
+++ b/MatrixSample.xlsx
@@ -5,35 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\WAPORIDOR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Python\WAPORIDOR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB6818A6-0E19-4A26-8322-C744BD468164}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224A81CD-C44A-4EE5-A296-541A672E1437}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F44BEC13-7B8F-4D7B-8CEE-7E5C263BCD0D}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{F44BEC13-7B8F-4D7B-8CEE-7E5C263BCD0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>y=</t>
   </si>
@@ -41,7 +33,10 @@
     <t>x=</t>
   </si>
   <si>
-    <t>2,3</t>
+    <t>y2 =</t>
+  </si>
+  <si>
+    <t>x2 =</t>
   </si>
 </sst>
 </file>
@@ -444,19 +439,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77BD3B24-F556-4448-BA95-D11A83363A37}">
   <dimension ref="B7:V21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83984375" bestFit="1" customWidth="1"/>
     <col min="3" max="9" width="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="19" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="19" width="3.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="11:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="11:22" x14ac:dyDescent="0.55000000000000004">
       <c r="K7">
         <v>0</v>
       </c>
@@ -492,9 +487,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="11:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="11:22" x14ac:dyDescent="0.55000000000000004">
       <c r="K8">
-        <f>S7+1</f>
+        <f t="shared" ref="K8:K15" si="1">S7+1</f>
         <v>9</v>
       </c>
       <c r="L8">
@@ -502,37 +497,37 @@
         <v>10</v>
       </c>
       <c r="M8">
-        <f t="shared" ref="M8:S8" si="1">L8+1</f>
+        <f t="shared" ref="M8:S8" si="2">L8+1</f>
         <v>11</v>
       </c>
       <c r="N8">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="11:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="K9">
         <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="R8">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="S8">
-        <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="11:22" x14ac:dyDescent="0.25">
-      <c r="K9">
-        <f>S8+1</f>
         <v>18</v>
       </c>
       <c r="L9">
@@ -540,69 +535,69 @@
         <v>19</v>
       </c>
       <c r="M9">
-        <f t="shared" ref="M9:S9" si="2">L9+1</f>
+        <f t="shared" ref="M9:S9" si="3">L9+1</f>
         <v>20</v>
       </c>
       <c r="N9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="O9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="P9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="R9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="S9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="11:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="11:22" x14ac:dyDescent="0.55000000000000004">
       <c r="K10">
-        <f>S9+1</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="L10">
-        <f t="shared" ref="L10:S13" si="3">K10+1</f>
+        <f t="shared" ref="L10:S13" si="4">K10+1</f>
         <v>28</v>
       </c>
       <c r="M10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="N10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="O10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="P10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
       <c r="R10">
-        <f t="shared" si="3"/>
+        <f>Q10+1</f>
         <v>34</v>
       </c>
       <c r="S10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="U10">
@@ -612,225 +607,252 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="11:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="11:22" x14ac:dyDescent="0.55000000000000004">
       <c r="K11">
-        <f>S10+1</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="L11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="M11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>38</v>
       </c>
       <c r="N11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39</v>
       </c>
       <c r="O11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="P11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
       <c r="R11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
       <c r="S11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="11:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="11:22" x14ac:dyDescent="0.55000000000000004">
       <c r="K12">
-        <f>S11+1</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="L12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>46</v>
       </c>
       <c r="M12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>47</v>
       </c>
       <c r="N12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
       <c r="O12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>49</v>
       </c>
       <c r="P12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>51</v>
       </c>
       <c r="R12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
       <c r="S12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="11:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="11:22" x14ac:dyDescent="0.55000000000000004">
       <c r="K13">
-        <f>S12+1</f>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="L13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>55</v>
       </c>
       <c r="M13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>56</v>
       </c>
       <c r="N13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>57</v>
       </c>
       <c r="O13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>58</v>
       </c>
       <c r="P13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>59</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="R13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>61</v>
       </c>
       <c r="S13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="11:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="11:22" x14ac:dyDescent="0.55000000000000004">
       <c r="K14">
-        <f>S13+1</f>
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="L14">
-        <f t="shared" ref="L14:S14" si="4">K14+1</f>
+        <f t="shared" ref="L14:S14" si="5">K14+1</f>
         <v>64</v>
       </c>
       <c r="M14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65</v>
       </c>
       <c r="N14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>66</v>
       </c>
       <c r="O14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>67</v>
       </c>
       <c r="P14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>68</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>69</v>
       </c>
       <c r="R14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>70</v>
       </c>
       <c r="S14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="11:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="11:22" x14ac:dyDescent="0.55000000000000004">
       <c r="K15">
-        <f>S14+1</f>
+        <f t="shared" si="1"/>
         <v>72</v>
       </c>
       <c r="L15">
-        <f t="shared" ref="L15:S15" si="5">K15+1</f>
+        <f t="shared" ref="L15:S15" si="6">K15+1</f>
         <v>73</v>
       </c>
       <c r="M15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>74</v>
       </c>
       <c r="N15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>75</v>
       </c>
       <c r="O15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>76</v>
       </c>
       <c r="P15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>77</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>78</v>
       </c>
       <c r="R15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>79</v>
       </c>
       <c r="S15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
         <v>0</v>
       </c>
       <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="K18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>16</v>
+      </c>
+      <c r="N18" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <f>L18/2</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" t="s">
         <v>1</v>
       </c>
       <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="K19" t="s">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>14</v>
+      </c>
+      <c r="N19" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <f>L19/2</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B20">
         <f>(((C18-1)*9)+C19)/2</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B21">
         <f>B20+9</f>
-        <v>19</v>
-      </c>
-      <c r="J21" t="s">
-        <v>2</v>
+        <v>4.5</v>
+      </c>
+      <c r="J21">
+        <f>O19*9+O18</f>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>